<commit_message>
Using neural network. Better results removing "outliers", actually special keys, from pressed key
</commit_message>
<xml_diff>
--- a/webService/sample.xlsx
+++ b/webService/sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>K-NN</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Random Forest</t>
   </si>
   <si>
+    <t>Neural Network - MPL</t>
+  </si>
+  <si>
     <t>Users</t>
   </si>
   <si>
@@ -43,115 +46,124 @@
     <t>Standard Deviation</t>
   </si>
   <si>
+    <t xml:space="preserve">   80.00%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   17.92%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   55.38%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   23.83%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   72.31%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   16.94%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4.65%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   81.54%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   18.52%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   83.08%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   11.13%</t>
+  </si>
+  <si>
     <t xml:space="preserve">   87.69%</t>
   </si>
   <si>
-    <t xml:space="preserve">   13.03%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   38.46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   18.94%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   81.54%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   12.64%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   80.00%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    4.65%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   20.49%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   11.57%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   12.78%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   64.62%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   22.92%</t>
+    <t xml:space="preserve">    9.67%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   69.23%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   14.44%</t>
   </si>
   <si>
     <t xml:space="preserve">   89.23%</t>
   </si>
   <si>
-    <t xml:space="preserve">   10.31%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   14.35%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   15.47%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   69.23%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   32.25%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   20.30%</t>
+    <t xml:space="preserve">   16.52%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   16.78%</t>
   </si>
   <si>
     <t xml:space="preserve">   86.15%</t>
   </si>
   <si>
-    <t xml:space="preserve">   12.45%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   93.85%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    7.45%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   16.28%</t>
+    <t xml:space="preserve">   15.63%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   19.73%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   78.46%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   27.61%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   15.86%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   14.33%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   19.57%</t>
   </si>
   <si>
     <t xml:space="preserve">   90.77%</t>
   </si>
   <si>
-    <t xml:space="preserve">   11.53%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   78.46%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   22.29%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   14.26%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   11.13%</t>
+    <t xml:space="preserve">    9.79%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   16.86%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   12.66%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   19.35%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.55%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   84.62%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   13.99%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   15.10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   63.08%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   22.58%</t>
   </si>
   <si>
     <t xml:space="preserve">   70.77%</t>
   </si>
   <si>
-    <t xml:space="preserve">   16.37%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   75.38%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   14.92%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   11.76%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   13.75%</t>
+    <t xml:space="preserve">   19.00%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    9.90%</t>
   </si>
 </sst>
 </file>
@@ -488,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,7 +508,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -515,251 +527,290 @@
       <c r="L1" t="s">
         <v>5</v>
       </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
       <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
       <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
-        <v>7</v>
-      </c>
       <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" t="s">
-        <v>7</v>
-      </c>
       <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
         <v>8</v>
       </c>
+      <c r="O2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:15">
       <c r="A3" t="n">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
         <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="M3" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:15">
       <c r="A4" t="n">
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I4" t="s">
         <v>16</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="M4" t="s">
-        <v>10</v>
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:15">
       <c r="A5" t="n">
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
       </c>
       <c r="J5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" t="s">
         <v>28</v>
       </c>
-      <c r="L5" t="s">
-        <v>29</v>
-      </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="N5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:15">
       <c r="A6" t="n">
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I6" t="s">
         <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L6" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="M6" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="N6" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:15">
       <c r="A7" t="n">
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="I7" t="s">
         <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="K7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L7" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="N7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>